<commit_message>
wg() only takes 'df' and 'tb'
Former-commit-id: 74c410f8273ca5d5df729bafa8877f5e89fc5e29
Former-commit-id: aee910d0aa3be019412fef3dbe9169175838ec4d
</commit_message>
<xml_diff>
--- a/tests/test_tax_transfers/test_data/test_dfs_wg.xlsx
+++ b/tests/test_tax_transfers/test_data/test_dfs_wg.xlsx
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="AD2" s="13">
         <f>1.15*(AQ2-((AK2+(AL2*AQ2)+(AM2*AP2))*AP2))</f>
-        <v>60.43528875000009</v>
+        <v>58.489817777777859</v>
       </c>
       <c r="AF2">
         <v>0.3</v>
@@ -1026,8 +1026,8 @@
         <v>100</v>
       </c>
       <c r="AJ2" s="12">
-        <f>MAX(ROUND((1-AF2)*MAX(0,AH2-AI2)+4,-1)-5,0)</f>
-        <v>1445</v>
+        <f>MAX((1-AF2)*(AH2-AI2),0)</f>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AK2">
         <v>0.02</v>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="AP2" s="12">
         <f>AJ2</f>
-        <v>1445</v>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AQ2">
-        <f>ROUND(MAX(MIN(I2,AN2),AO2)+4,-1)-5</f>
-        <v>565</v>
+        <f>MIN(MAX(I2,AO2),AN2)</f>
+        <v>563</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="AD3" s="13">
         <f t="shared" ref="AD3:AD4" si="1">1.15*(AQ3-((AK3+(AL3*AQ3)+(AM3*AP3))*AP3))</f>
-        <v>60.43528875000009</v>
+        <v>58.489817777777859</v>
       </c>
       <c r="AF3">
         <v>0.3</v>
@@ -1161,8 +1161,8 @@
         <v>100</v>
       </c>
       <c r="AJ3" s="12">
-        <f t="shared" ref="AJ3:AJ13" si="3">MAX(ROUND((1-AF3)*MAX(0,AH3-AI3)+4,-1)-5,0)</f>
-        <v>1445</v>
+        <f t="shared" ref="AJ3:AJ13" si="3">MAX((1-AF3)*(AH3-AI3),0)</f>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AK3">
         <v>0.02</v>
@@ -1181,11 +1181,11 @@
       </c>
       <c r="AP3" s="12">
         <f t="shared" ref="AP3:AP8" si="4">AJ3</f>
-        <v>1445</v>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AQ3">
-        <f t="shared" ref="AQ3:AQ13" si="5">ROUND(MAX(MIN(I3,AN3),AO3)+4,-1)-5</f>
-        <v>565</v>
+        <f t="shared" ref="AQ3:AQ13" si="5">MIN(MAX(I3,AO3),AN3)</f>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="AD4" s="13">
         <f t="shared" si="1"/>
-        <v>60.43528875000009</v>
+        <v>58.489817777777859</v>
       </c>
       <c r="AF4">
         <v>0.3</v>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="AJ4" s="12">
         <f t="shared" si="3"/>
-        <v>1445</v>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AK4">
         <v>0.02</v>
@@ -1316,11 +1316,11 @@
       </c>
       <c r="AP4" s="12">
         <f t="shared" si="4"/>
-        <v>1445</v>
+        <v>1446.6666666666665</v>
       </c>
       <c r="AQ4">
         <f t="shared" si="5"/>
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="AD5" s="13">
         <f>1.08*(AQ5-((AK5+(AL5*AQ5)+(AM5*AP5))*AP5))</f>
-        <v>191.51471817000001</v>
+        <v>194.17440000000002</v>
       </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="AJ5" s="12">
         <f t="shared" si="3"/>
-        <v>665</v>
+        <v>666.66666666666674</v>
       </c>
       <c r="AK5" s="9">
         <v>5.7000000000000002E-2</v>
@@ -1452,11 +1452,11 @@
       </c>
       <c r="AP5" s="12">
         <f t="shared" si="4"/>
-        <v>665</v>
+        <v>666.66666666666674</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="AD6" s="13">
         <f>1.08*(AQ6-((AK6+(AL6*AQ6)+(AM6*AP6))*AP6))</f>
-        <v>191.51471817000001</v>
+        <v>194.17440000000002</v>
       </c>
       <c r="AF6" s="3">
         <v>0.2</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="AJ6" s="12">
         <f t="shared" si="3"/>
-        <v>665</v>
+        <v>666.66666666666674</v>
       </c>
       <c r="AK6" s="6">
         <v>5.7000000000000002E-2</v>
@@ -1587,11 +1587,11 @@
       </c>
       <c r="AP6" s="12">
         <f t="shared" si="4"/>
-        <v>665</v>
+        <v>666.66666666666674</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="AD7" s="13">
         <f t="shared" ref="AD7:AD8" si="6">1.08*(AQ7-((AK7+(AL7*AQ7)+(AM7*AP7))*AP7))</f>
-        <v>15.962717249999999</v>
+        <v>18.784535520000077</v>
       </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="AJ7" s="12">
         <f t="shared" si="3"/>
-        <v>1075</v>
+        <v>1073.3333333333333</v>
       </c>
       <c r="AK7" s="9">
         <v>5.7000000000000002E-2</v>
@@ -1723,11 +1723,11 @@
       </c>
       <c r="AP7" s="12">
         <f t="shared" si="4"/>
-        <v>1075</v>
+        <v>1073.3333333333333</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="AD8" s="13">
         <f t="shared" si="6"/>
-        <v>15.962717249999999</v>
+        <v>18.784535520000077</v>
       </c>
       <c r="AF8" s="3">
         <v>0.3</v>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="AJ8" s="12">
         <f t="shared" si="3"/>
-        <v>1075</v>
+        <v>1073.3333333333333</v>
       </c>
       <c r="AK8" s="6">
         <v>5.7000000000000002E-2</v>
@@ -1858,11 +1858,11 @@
       </c>
       <c r="AP8" s="12">
         <f t="shared" si="4"/>
-        <v>1075</v>
+        <v>1073.3333333333333</v>
       </c>
       <c r="AQ8">
         <f t="shared" si="5"/>
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="AD9" s="13">
         <f>(AQ9-((AK9+(AL9*AQ9)+(AM9*AP9))*AP9))</f>
-        <v>504.25435025000002</v>
+        <v>508.75845025000001</v>
       </c>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="AQ9">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="AD10" s="13">
         <f t="shared" ref="AD10:AD13" si="7">(AQ10-((AK10+(AL10*AQ10)+(AM10*AP10))*AP10))</f>
-        <v>504.25435025000002</v>
+        <v>508.75845025000001</v>
       </c>
       <c r="AF10" s="3">
         <v>0.1</v>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="AQ10">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="AD11" s="13">
         <f t="shared" si="7"/>
-        <v>504.25435025000002</v>
+        <v>508.75845025000001</v>
       </c>
       <c r="AF11" s="3">
         <v>0.1</v>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="AQ11">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="AD12" s="13">
         <f t="shared" si="7"/>
-        <v>504.25435025000002</v>
+        <v>508.75845025000001</v>
       </c>
       <c r="AF12" s="3">
         <v>0.1</v>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="AQ12">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="AD13" s="13">
         <f t="shared" si="7"/>
-        <v>504.25435025000002</v>
+        <v>508.75845025000001</v>
       </c>
       <c r="AF13" s="3">
         <v>0.1</v>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="AQ13">
         <f t="shared" si="5"/>
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">

</xml_diff>